<commit_message>
Update test data to match full service import
</commit_message>
<xml_diff>
--- a/tests/assets/services_import_1_good.xlsx
+++ b/tests/assets/services_import_1_good.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">organisation_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -43,39 +40,117 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">wait_time</t>
+  </si>
+  <si>
     <t xml:space="preserve">is_free</t>
   </si>
   <si>
+    <t xml:space="preserve">fees_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fees_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testimonial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video_embed</t>
+  </si>
+  <si>
     <t xml:space="preserve">url</t>
   </si>
   <si>
+    <t xml:space="preserve">contact_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_email</t>
+  </si>
+  <si>
     <t xml:space="preserve">show_referral_disclaimer</t>
   </si>
   <si>
     <t xml:space="preserve">referral_method</t>
   </si>
   <si>
-    <t xml:space="preserve">Decentralized human-resource instruction set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
+    <t xml:space="preserve">referral_button_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">referral_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">referral_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_age_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_employment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criteria_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seamless 24 hour system engine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">advice</t>
   </si>
   <si>
     <t xml:space="preserve">inactive</t>
   </si>
   <si>
-    <t xml:space="preserve">Phasellus in felis.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suspendisse potenti. In eleifend quam a odio. In hac habitasse platea dictumst.
-Maecenas ut massa quis augue luctus tincidunt. Nulla mollis molestie lorem. Quisque ut erat.
-Curabitur gravida nisi at nibh. In hac habitasse platea dictumst. Aliquam augue quam, sollicitudin vitae, consectetuer eget, rutrum at, lorem.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://yolasite.com/nunc/proin/at/turpis/a/pede.js</t>
-  </si>
-  <si>
-    <t xml:space="preserve">external</t>
+    <t xml:space="preserve">Proin interdum mauris non ligula pellentesque ultrices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aenean fermentum. Donec ut mauris eget massa tempor convallis. Nulla neque libero, convallis eget, eleifend luctus, ultricies eu, nibh.
+Quisque id justo sit amet sapien dignissim vestibulum. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Nulla dapibus dolor vel est. Donec odio justo, sollicitudin ut, suscipit a, feugiat et, eros.
+Vestibulum ac est lacinia nisi venenatis tristique. Fusce congue, diam id ornare imperdiet, sapien urna pretium nisl, ut volutpat sapien arcu sed augue. Aliquam erat volutpat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quisque ut erat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://over-blog.com/lectus/pellentesque/eget/nunc/donec/quis/orci.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://cmu.edu/dolor.jsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo ann Timothy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jann0@ebay.co.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cras in purus eu magna vulputate luctus. Cum sociis natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sed ante. Vivamus tortor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Praesent lectus. Vestibulum quam sapien, varius ut, blandit non, interdum in, ante.</t>
   </si>
 </sst>
 </file>
@@ -190,26 +265,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="125.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="7.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="45.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="58.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="89.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="63.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="9.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,43 +337,124 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
+      <c r="R2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Permission for importing services passed
</commit_message>
<xml_diff>
--- a/tests/assets/services_import_1_good.xlsx
+++ b/tests/assets/services_import_1_good.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Seamless 24 hour system engine</t>
   </si>
   <si>
-    <t xml:space="preserve">advice</t>
+    <t xml:space="preserve">service</t>
   </si>
   <si>
     <t xml:space="preserve">inactive</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">jann0@ebay.co.uk</t>
   </si>
   <si>
-    <t xml:space="preserve">internal</t>
+    <t xml:space="preserve">none</t>
   </si>
   <si>
     <t xml:space="preserve">Cras in purus eu magna vulputate luctus. Cum sociis natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus.</t>
@@ -165,6 +165,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -255,7 +256,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -268,7 +269,7 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,24 +281,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="45.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="58.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="89.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="63.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="9.45"/>
@@ -434,7 +435,7 @@
         <v>38</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>39</v>

</xml_diff>